<commit_message>
Add test coverage for serializing non-eloquent queries
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/from-query-store-with-eager-loads.xlsx
+++ b/tests/Data/Disks/Local/from-query-store-with-eager-loads.xlsx
@@ -17,307 +17,307 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
-    <t>Prof. Bertha Torphy DDS</t>
+    <t>Juvenal Bashirian V</t>
   </si>
   <si>
     <t>Group 1</t>
   </si>
   <si>
-    <t>Miss Fabiola Walsh</t>
-  </si>
-  <si>
-    <t>Katrina Lakin</t>
-  </si>
-  <si>
-    <t>Ms. Paige Jacobson I</t>
-  </si>
-  <si>
-    <t>Karelle Lindgren</t>
-  </si>
-  <si>
-    <t>Vicenta Nienow I</t>
-  </si>
-  <si>
-    <t>Mrs. Corine Kirlin MD</t>
-  </si>
-  <si>
-    <t>Dr. Hadley Dach</t>
-  </si>
-  <si>
-    <t>Natalia Kertzmann</t>
-  </si>
-  <si>
-    <t>Alice Jacobi</t>
-  </si>
-  <si>
-    <t>Kristofer Witting</t>
-  </si>
-  <si>
-    <t>Brisa Mertz</t>
-  </si>
-  <si>
-    <t>Andres Veum</t>
-  </si>
-  <si>
-    <t>Walker Hills</t>
-  </si>
-  <si>
-    <t>Dr. Alexandrine Schuster</t>
-  </si>
-  <si>
-    <t>Kelly Considine</t>
-  </si>
-  <si>
-    <t>Edmund Howe</t>
-  </si>
-  <si>
-    <t>Travis Donnelly</t>
-  </si>
-  <si>
-    <t>Dr. Dennis Bradtke PhD</t>
-  </si>
-  <si>
-    <t>Brooklyn Schmidt MD</t>
-  </si>
-  <si>
-    <t>Bria Armstrong</t>
-  </si>
-  <si>
-    <t>Russ Hettinger III</t>
-  </si>
-  <si>
-    <t>Demetris Yundt I</t>
-  </si>
-  <si>
-    <t>Rachelle Prosacco</t>
-  </si>
-  <si>
-    <t>Mrs. Melba Hand</t>
-  </si>
-  <si>
-    <t>Prof. Kenna Balistreri II</t>
-  </si>
-  <si>
-    <t>Dr. Gaylord Heidenreich I</t>
-  </si>
-  <si>
-    <t>Ms. Heloise Hammes</t>
-  </si>
-  <si>
-    <t>Jessica Bailey</t>
-  </si>
-  <si>
-    <t>Russel Davis</t>
-  </si>
-  <si>
-    <t>Jaylan Keebler</t>
-  </si>
-  <si>
-    <t>Miss Ana Powlowski</t>
-  </si>
-  <si>
-    <t>Nash Homenick</t>
-  </si>
-  <si>
-    <t>Myah Hermann</t>
-  </si>
-  <si>
-    <t>Merlin Hegmann IV</t>
-  </si>
-  <si>
-    <t>Mrs. Sophia Kunze</t>
-  </si>
-  <si>
-    <t>Esmeralda Ratke</t>
-  </si>
-  <si>
-    <t>Mrs. River Glover Sr.</t>
-  </si>
-  <si>
-    <t>Andreane Okuneva</t>
-  </si>
-  <si>
-    <t>Ms. Kianna Stokes PhD</t>
-  </si>
-  <si>
-    <t>Teresa Jast</t>
-  </si>
-  <si>
-    <t>Lorenzo Rohan</t>
-  </si>
-  <si>
-    <t>Guiseppe Morar</t>
-  </si>
-  <si>
-    <t>Vincenza Rohan</t>
-  </si>
-  <si>
-    <t>Vesta Collins</t>
-  </si>
-  <si>
-    <t>Kallie Rolfson</t>
-  </si>
-  <si>
-    <t>Miss Priscilla Wehner PhD</t>
-  </si>
-  <si>
-    <t>Dr. Rocky Feil</t>
-  </si>
-  <si>
-    <t>Cathrine Donnelly</t>
-  </si>
-  <si>
-    <t>Wava Kassulke III</t>
-  </si>
-  <si>
-    <t>Prof. Ivah Wiegand</t>
-  </si>
-  <si>
-    <t>Lemuel Walter</t>
-  </si>
-  <si>
-    <t>Miss Abagail Carroll</t>
-  </si>
-  <si>
-    <t>Prof. Perry Schaden DDS</t>
-  </si>
-  <si>
-    <t>Stone Leuschke III</t>
-  </si>
-  <si>
-    <t>Donny Ryan</t>
-  </si>
-  <si>
-    <t>Mrs. Jessica Skiles IV</t>
-  </si>
-  <si>
-    <t>Gardner Willms</t>
-  </si>
-  <si>
-    <t>Dr. Delbert McCullough II</t>
-  </si>
-  <si>
-    <t>Alize Johnson</t>
-  </si>
-  <si>
-    <t>Dr. Khalil Ratke I</t>
-  </si>
-  <si>
-    <t>Vincenza Baumbach IV</t>
-  </si>
-  <si>
-    <t>Berta Crooks</t>
-  </si>
-  <si>
-    <t>Dr. Jaquan Reinger V</t>
-  </si>
-  <si>
-    <t>Aric Schaden</t>
-  </si>
-  <si>
-    <t>Miles Crona</t>
-  </si>
-  <si>
-    <t>Marcelina Pfannerstill</t>
-  </si>
-  <si>
-    <t>Brooks Waelchi</t>
-  </si>
-  <si>
-    <t>Bruce Purdy</t>
-  </si>
-  <si>
-    <t>Vincenzo D'Amore</t>
-  </si>
-  <si>
-    <t>Lisa Schamberger</t>
-  </si>
-  <si>
-    <t>Daron Nicolas</t>
-  </si>
-  <si>
-    <t>Glenda Jaskolski V</t>
-  </si>
-  <si>
-    <t>Dr. Regan McLaughlin II</t>
-  </si>
-  <si>
-    <t>Garett Willms</t>
-  </si>
-  <si>
-    <t>Miss Vilma Mueller</t>
-  </si>
-  <si>
-    <t>Mr. Layne Grant</t>
-  </si>
-  <si>
-    <t>Kristian Braun DVM</t>
-  </si>
-  <si>
-    <t>Loren Boyer</t>
-  </si>
-  <si>
-    <t>Devan Jaskolski</t>
-  </si>
-  <si>
-    <t>Dr. Vicente Bednar I</t>
-  </si>
-  <si>
-    <t>Blanche Bartoletti</t>
-  </si>
-  <si>
-    <t>Crystal Bechtelar</t>
-  </si>
-  <si>
-    <t>Sasha Eichmann</t>
-  </si>
-  <si>
-    <t>Tiana Kris</t>
-  </si>
-  <si>
-    <t>Tommie Breitenberg V</t>
-  </si>
-  <si>
-    <t>Miss Flo Littel</t>
-  </si>
-  <si>
-    <t>Ara Rempel</t>
-  </si>
-  <si>
-    <t>Francesca Stehr</t>
-  </si>
-  <si>
-    <t>Dr. Blaise Rosenbaum</t>
-  </si>
-  <si>
-    <t>Miss Alejandra Davis</t>
-  </si>
-  <si>
-    <t>Pierce Rodriguez DVM</t>
-  </si>
-  <si>
-    <t>Cyrus Trantow DVM</t>
-  </si>
-  <si>
-    <t>Scot O'Connell</t>
-  </si>
-  <si>
-    <t>Ms. Elyssa Huels</t>
-  </si>
-  <si>
-    <t>Ella Leannon</t>
-  </si>
-  <si>
-    <t>Prof. Scotty Lindgren DDS</t>
-  </si>
-  <si>
-    <t>Mr. Josiah Kulas Sr.</t>
-  </si>
-  <si>
-    <t>Lillie Raynor</t>
-  </si>
-  <si>
-    <t>Prof. Marisa Bartell II</t>
+    <t>Ramon Borer</t>
+  </si>
+  <si>
+    <t>Donna Haley</t>
+  </si>
+  <si>
+    <t>Jerel Ledner</t>
+  </si>
+  <si>
+    <t>Jesse Boehm</t>
+  </si>
+  <si>
+    <t>Concepcion Tremblay</t>
+  </si>
+  <si>
+    <t>Green Bosco</t>
+  </si>
+  <si>
+    <t>Ignacio Dickens</t>
+  </si>
+  <si>
+    <t>Lonie McKenzie</t>
+  </si>
+  <si>
+    <t>Mrs. Tessie Stanton</t>
+  </si>
+  <si>
+    <t>Raven Sipes</t>
+  </si>
+  <si>
+    <t>Vladimir Schaden</t>
+  </si>
+  <si>
+    <t>Amelie Renner</t>
+  </si>
+  <si>
+    <t>Mr. Chauncey Flatley Jr.</t>
+  </si>
+  <si>
+    <t>Rogelio Stokes</t>
+  </si>
+  <si>
+    <t>Mr. Giovani Lemke III</t>
+  </si>
+  <si>
+    <t>Zoie Batz</t>
+  </si>
+  <si>
+    <t>Ms. Elinor Bartell</t>
+  </si>
+  <si>
+    <t>Una Erdman V</t>
+  </si>
+  <si>
+    <t>Fletcher Parisian</t>
+  </si>
+  <si>
+    <t>Carey Sawayn</t>
+  </si>
+  <si>
+    <t>Deontae Lynch</t>
+  </si>
+  <si>
+    <t>Dallas Lemke Sr.</t>
+  </si>
+  <si>
+    <t>Cali Bartoletti</t>
+  </si>
+  <si>
+    <t>Shyanne Hagenes</t>
+  </si>
+  <si>
+    <t>Lyda Welch</t>
+  </si>
+  <si>
+    <t>Bradley Purdy</t>
+  </si>
+  <si>
+    <t>Prof. Dennis Shields IV</t>
+  </si>
+  <si>
+    <t>Thomas Romaguera</t>
+  </si>
+  <si>
+    <t>Greyson Runte</t>
+  </si>
+  <si>
+    <t>Ladarius Rippin</t>
+  </si>
+  <si>
+    <t>Miss Kayla Stark</t>
+  </si>
+  <si>
+    <t>Bridgette Halvorson</t>
+  </si>
+  <si>
+    <t>Elwyn Will</t>
+  </si>
+  <si>
+    <t>Leilani Luettgen</t>
+  </si>
+  <si>
+    <t>Dr. Fiona Hackett</t>
+  </si>
+  <si>
+    <t>Mr. Saige Buckridge</t>
+  </si>
+  <si>
+    <t>Alexandrea Schmidt</t>
+  </si>
+  <si>
+    <t>Dusty Cruickshank</t>
+  </si>
+  <si>
+    <t>Joannie Jenkins</t>
+  </si>
+  <si>
+    <t>Prof. Maximillian Wintheiser Sr.</t>
+  </si>
+  <si>
+    <t>Ronny West</t>
+  </si>
+  <si>
+    <t>June Emard</t>
+  </si>
+  <si>
+    <t>Harley Ortiz</t>
+  </si>
+  <si>
+    <t>Daphne Runolfsdottir</t>
+  </si>
+  <si>
+    <t>Penelope Schneider</t>
+  </si>
+  <si>
+    <t>Deion Parker MD</t>
+  </si>
+  <si>
+    <t>Fannie Waelchi Jr.</t>
+  </si>
+  <si>
+    <t>Ms. Rosalind Schiller</t>
+  </si>
+  <si>
+    <t>Cheyanne Schaefer</t>
+  </si>
+  <si>
+    <t>Guido Olson II</t>
+  </si>
+  <si>
+    <t>Ms. Rosalind Vandervort V</t>
+  </si>
+  <si>
+    <t>Christop McLaughlin</t>
+  </si>
+  <si>
+    <t>Nikki Walker</t>
+  </si>
+  <si>
+    <t>Carmine O'Conner</t>
+  </si>
+  <si>
+    <t>Kendra Larson</t>
+  </si>
+  <si>
+    <t>Maximillian Stiedemann</t>
+  </si>
+  <si>
+    <t>Maverick Weimann</t>
+  </si>
+  <si>
+    <t>Effie Klein</t>
+  </si>
+  <si>
+    <t>Einar Huels</t>
+  </si>
+  <si>
+    <t>Adela Murazik</t>
+  </si>
+  <si>
+    <t>Osborne Ferry</t>
+  </si>
+  <si>
+    <t>Burnice Marquardt</t>
+  </si>
+  <si>
+    <t>Yolanda Legros II</t>
+  </si>
+  <si>
+    <t>Christian Herzog</t>
+  </si>
+  <si>
+    <t>Mr. Darius Mills</t>
+  </si>
+  <si>
+    <t>Jordy Davis</t>
+  </si>
+  <si>
+    <t>Gabriel Paucek V</t>
+  </si>
+  <si>
+    <t>Jordon Thompson</t>
+  </si>
+  <si>
+    <t>Ova Volkman</t>
+  </si>
+  <si>
+    <t>Florida Abernathy</t>
+  </si>
+  <si>
+    <t>Delmer Jakubowski IV</t>
+  </si>
+  <si>
+    <t>Jacques Mitchell</t>
+  </si>
+  <si>
+    <t>Mr. Geovanny Howe</t>
+  </si>
+  <si>
+    <t>Marjorie Denesik I</t>
+  </si>
+  <si>
+    <t>Hanna Ledner Sr.</t>
+  </si>
+  <si>
+    <t>Miss Frieda Walker I</t>
+  </si>
+  <si>
+    <t>Dr. Alena Borer</t>
+  </si>
+  <si>
+    <t>Gavin Flatley</t>
+  </si>
+  <si>
+    <t>Zula McDermott</t>
+  </si>
+  <si>
+    <t>Rosamond Gaylord</t>
+  </si>
+  <si>
+    <t>Ms. Shyanne Bailey Jr.</t>
+  </si>
+  <si>
+    <t>Prof. Abbigail Green MD</t>
+  </si>
+  <si>
+    <t>Terrill Marvin</t>
+  </si>
+  <si>
+    <t>Prof. Carmine Prohaska</t>
+  </si>
+  <si>
+    <t>Lelah Pfannerstill</t>
+  </si>
+  <si>
+    <t>Dr. Titus Toy</t>
+  </si>
+  <si>
+    <t>Jayde O'Connell</t>
+  </si>
+  <si>
+    <t>Vallie Goodwin</t>
+  </si>
+  <si>
+    <t>Dr. Amparo Gaylord DVM</t>
+  </si>
+  <si>
+    <t>Ms. Josefa Pouros</t>
+  </si>
+  <si>
+    <t>Russ Keebler</t>
+  </si>
+  <si>
+    <t>Prof. Malachi Russel Sr.</t>
+  </si>
+  <si>
+    <t>Dr. Zion Simonis Sr.</t>
+  </si>
+  <si>
+    <t>Beth Farrell</t>
+  </si>
+  <si>
+    <t>Sanford Medhurst DDS</t>
+  </si>
+  <si>
+    <t>Mrs. Alicia Armstrong MD</t>
+  </si>
+  <si>
+    <t>Mckenna Gulgowski</t>
+  </si>
+  <si>
+    <t>Mollie Ondricka</t>
+  </si>
+  <si>
+    <t>Scot Will I</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Improve failure skipping on row validation during batch import
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/from-query-store-with-eager-loads.xlsx
+++ b/tests/Data/Disks/Local/from-query-store-with-eager-loads.xlsx
@@ -17,307 +17,307 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="101">
   <si>
-    <t>Juvenal Bashirian V</t>
+    <t>Marjorie Mann</t>
   </si>
   <si>
     <t>Group 1</t>
   </si>
   <si>
-    <t>Ramon Borer</t>
-  </si>
-  <si>
-    <t>Donna Haley</t>
-  </si>
-  <si>
-    <t>Jerel Ledner</t>
-  </si>
-  <si>
-    <t>Jesse Boehm</t>
-  </si>
-  <si>
-    <t>Concepcion Tremblay</t>
-  </si>
-  <si>
-    <t>Green Bosco</t>
-  </si>
-  <si>
-    <t>Ignacio Dickens</t>
-  </si>
-  <si>
-    <t>Lonie McKenzie</t>
-  </si>
-  <si>
-    <t>Mrs. Tessie Stanton</t>
-  </si>
-  <si>
-    <t>Raven Sipes</t>
-  </si>
-  <si>
-    <t>Vladimir Schaden</t>
-  </si>
-  <si>
-    <t>Amelie Renner</t>
-  </si>
-  <si>
-    <t>Mr. Chauncey Flatley Jr.</t>
-  </si>
-  <si>
-    <t>Rogelio Stokes</t>
-  </si>
-  <si>
-    <t>Mr. Giovani Lemke III</t>
-  </si>
-  <si>
-    <t>Zoie Batz</t>
-  </si>
-  <si>
-    <t>Ms. Elinor Bartell</t>
-  </si>
-  <si>
-    <t>Una Erdman V</t>
-  </si>
-  <si>
-    <t>Fletcher Parisian</t>
-  </si>
-  <si>
-    <t>Carey Sawayn</t>
-  </si>
-  <si>
-    <t>Deontae Lynch</t>
-  </si>
-  <si>
-    <t>Dallas Lemke Sr.</t>
-  </si>
-  <si>
-    <t>Cali Bartoletti</t>
-  </si>
-  <si>
-    <t>Shyanne Hagenes</t>
-  </si>
-  <si>
-    <t>Lyda Welch</t>
-  </si>
-  <si>
-    <t>Bradley Purdy</t>
-  </si>
-  <si>
-    <t>Prof. Dennis Shields IV</t>
-  </si>
-  <si>
-    <t>Thomas Romaguera</t>
-  </si>
-  <si>
-    <t>Greyson Runte</t>
-  </si>
-  <si>
-    <t>Ladarius Rippin</t>
-  </si>
-  <si>
-    <t>Miss Kayla Stark</t>
-  </si>
-  <si>
-    <t>Bridgette Halvorson</t>
-  </si>
-  <si>
-    <t>Elwyn Will</t>
-  </si>
-  <si>
-    <t>Leilani Luettgen</t>
-  </si>
-  <si>
-    <t>Dr. Fiona Hackett</t>
-  </si>
-  <si>
-    <t>Mr. Saige Buckridge</t>
-  </si>
-  <si>
-    <t>Alexandrea Schmidt</t>
-  </si>
-  <si>
-    <t>Dusty Cruickshank</t>
-  </si>
-  <si>
-    <t>Joannie Jenkins</t>
-  </si>
-  <si>
-    <t>Prof. Maximillian Wintheiser Sr.</t>
-  </si>
-  <si>
-    <t>Ronny West</t>
-  </si>
-  <si>
-    <t>June Emard</t>
-  </si>
-  <si>
-    <t>Harley Ortiz</t>
-  </si>
-  <si>
-    <t>Daphne Runolfsdottir</t>
-  </si>
-  <si>
-    <t>Penelope Schneider</t>
-  </si>
-  <si>
-    <t>Deion Parker MD</t>
-  </si>
-  <si>
-    <t>Fannie Waelchi Jr.</t>
-  </si>
-  <si>
-    <t>Ms. Rosalind Schiller</t>
-  </si>
-  <si>
-    <t>Cheyanne Schaefer</t>
-  </si>
-  <si>
-    <t>Guido Olson II</t>
-  </si>
-  <si>
-    <t>Ms. Rosalind Vandervort V</t>
-  </si>
-  <si>
-    <t>Christop McLaughlin</t>
-  </si>
-  <si>
-    <t>Nikki Walker</t>
-  </si>
-  <si>
-    <t>Carmine O'Conner</t>
-  </si>
-  <si>
-    <t>Kendra Larson</t>
-  </si>
-  <si>
-    <t>Maximillian Stiedemann</t>
-  </si>
-  <si>
-    <t>Maverick Weimann</t>
-  </si>
-  <si>
-    <t>Effie Klein</t>
-  </si>
-  <si>
-    <t>Einar Huels</t>
-  </si>
-  <si>
-    <t>Adela Murazik</t>
-  </si>
-  <si>
-    <t>Osborne Ferry</t>
-  </si>
-  <si>
-    <t>Burnice Marquardt</t>
-  </si>
-  <si>
-    <t>Yolanda Legros II</t>
-  </si>
-  <si>
-    <t>Christian Herzog</t>
-  </si>
-  <si>
-    <t>Mr. Darius Mills</t>
-  </si>
-  <si>
-    <t>Jordy Davis</t>
-  </si>
-  <si>
-    <t>Gabriel Paucek V</t>
-  </si>
-  <si>
-    <t>Jordon Thompson</t>
-  </si>
-  <si>
-    <t>Ova Volkman</t>
-  </si>
-  <si>
-    <t>Florida Abernathy</t>
-  </si>
-  <si>
-    <t>Delmer Jakubowski IV</t>
-  </si>
-  <si>
-    <t>Jacques Mitchell</t>
-  </si>
-  <si>
-    <t>Mr. Geovanny Howe</t>
-  </si>
-  <si>
-    <t>Marjorie Denesik I</t>
-  </si>
-  <si>
-    <t>Hanna Ledner Sr.</t>
-  </si>
-  <si>
-    <t>Miss Frieda Walker I</t>
-  </si>
-  <si>
-    <t>Dr. Alena Borer</t>
-  </si>
-  <si>
-    <t>Gavin Flatley</t>
-  </si>
-  <si>
-    <t>Zula McDermott</t>
-  </si>
-  <si>
-    <t>Rosamond Gaylord</t>
-  </si>
-  <si>
-    <t>Ms. Shyanne Bailey Jr.</t>
-  </si>
-  <si>
-    <t>Prof. Abbigail Green MD</t>
-  </si>
-  <si>
-    <t>Terrill Marvin</t>
-  </si>
-  <si>
-    <t>Prof. Carmine Prohaska</t>
-  </si>
-  <si>
-    <t>Lelah Pfannerstill</t>
-  </si>
-  <si>
-    <t>Dr. Titus Toy</t>
-  </si>
-  <si>
-    <t>Jayde O'Connell</t>
-  </si>
-  <si>
-    <t>Vallie Goodwin</t>
-  </si>
-  <si>
-    <t>Dr. Amparo Gaylord DVM</t>
-  </si>
-  <si>
-    <t>Ms. Josefa Pouros</t>
-  </si>
-  <si>
-    <t>Russ Keebler</t>
-  </si>
-  <si>
-    <t>Prof. Malachi Russel Sr.</t>
-  </si>
-  <si>
-    <t>Dr. Zion Simonis Sr.</t>
-  </si>
-  <si>
-    <t>Beth Farrell</t>
-  </si>
-  <si>
-    <t>Sanford Medhurst DDS</t>
-  </si>
-  <si>
-    <t>Mrs. Alicia Armstrong MD</t>
-  </si>
-  <si>
-    <t>Mckenna Gulgowski</t>
-  </si>
-  <si>
-    <t>Mollie Ondricka</t>
-  </si>
-  <si>
-    <t>Scot Will I</t>
+    <t>Mrs. Kathryne Shanahan IV</t>
+  </si>
+  <si>
+    <t>Isabel Satterfield</t>
+  </si>
+  <si>
+    <t>Junius Christiansen</t>
+  </si>
+  <si>
+    <t>Mr. Lon Marquardt Jr.</t>
+  </si>
+  <si>
+    <t>Virgie Feest</t>
+  </si>
+  <si>
+    <t>Roderick Eichmann</t>
+  </si>
+  <si>
+    <t>Raleigh Lynch</t>
+  </si>
+  <si>
+    <t>Prof. Jerry Murray</t>
+  </si>
+  <si>
+    <t>Guy Farrell</t>
+  </si>
+  <si>
+    <t>Dr. Edwardo Heaney III</t>
+  </si>
+  <si>
+    <t>Valentine Kub</t>
+  </si>
+  <si>
+    <t>Zola Lehner</t>
+  </si>
+  <si>
+    <t>Mark Marvin</t>
+  </si>
+  <si>
+    <t>Earl Tillman Sr.</t>
+  </si>
+  <si>
+    <t>Ottilie Treutel</t>
+  </si>
+  <si>
+    <t>Kenton Dickens</t>
+  </si>
+  <si>
+    <t>Moises Wunsch</t>
+  </si>
+  <si>
+    <t>Dr. Ena Pouros PhD</t>
+  </si>
+  <si>
+    <t>Miss Adrienne Olson</t>
+  </si>
+  <si>
+    <t>Prof. Kieran Roob Jr.</t>
+  </si>
+  <si>
+    <t>Agustin Gutmann</t>
+  </si>
+  <si>
+    <t>Mrs. Marisol O'Conner</t>
+  </si>
+  <si>
+    <t>Parker Kreiger</t>
+  </si>
+  <si>
+    <t>Linnie Stoltenberg Jr.</t>
+  </si>
+  <si>
+    <t>Bulah Davis</t>
+  </si>
+  <si>
+    <t>Nathanael Cole</t>
+  </si>
+  <si>
+    <t>Emie Thiel</t>
+  </si>
+  <si>
+    <t>Jolie Eichmann</t>
+  </si>
+  <si>
+    <t>Miss Ofelia Bailey IV</t>
+  </si>
+  <si>
+    <t>Maxime Langworth</t>
+  </si>
+  <si>
+    <t>Jerrold Gutkowski</t>
+  </si>
+  <si>
+    <t>Dr. Kyla Haag</t>
+  </si>
+  <si>
+    <t>Lola Becker DVM</t>
+  </si>
+  <si>
+    <t>Lura Kuhic</t>
+  </si>
+  <si>
+    <t>Wendell Purdy</t>
+  </si>
+  <si>
+    <t>Meta Ruecker</t>
+  </si>
+  <si>
+    <t>Mr. Carson Flatley IV</t>
+  </si>
+  <si>
+    <t>Jakob Gorczany</t>
+  </si>
+  <si>
+    <t>Ms. Blanca Mueller</t>
+  </si>
+  <si>
+    <t>Damon Hoeger PhD</t>
+  </si>
+  <si>
+    <t>Leonie Mueller</t>
+  </si>
+  <si>
+    <t>Colby Koss</t>
+  </si>
+  <si>
+    <t>Samir Fadel</t>
+  </si>
+  <si>
+    <t>Prof. Jevon Sporer</t>
+  </si>
+  <si>
+    <t>Verner Gutkowski</t>
+  </si>
+  <si>
+    <t>Lillian Christiansen III</t>
+  </si>
+  <si>
+    <t>Lexie Morissette</t>
+  </si>
+  <si>
+    <t>Leone Miller</t>
+  </si>
+  <si>
+    <t>Gideon Klocko</t>
+  </si>
+  <si>
+    <t>Demario Waelchi</t>
+  </si>
+  <si>
+    <t>Jamel Gottlieb</t>
+  </si>
+  <si>
+    <t>Dayana Mosciski</t>
+  </si>
+  <si>
+    <t>Harley Donnelly DDS</t>
+  </si>
+  <si>
+    <t>Allie Hill</t>
+  </si>
+  <si>
+    <t>Miss Simone Larson IV</t>
+  </si>
+  <si>
+    <t>Kirk Kutch</t>
+  </si>
+  <si>
+    <t>Mr. Frederick Howe</t>
+  </si>
+  <si>
+    <t>Gwen Toy IV</t>
+  </si>
+  <si>
+    <t>Ms. Mabelle Hettinger</t>
+  </si>
+  <si>
+    <t>Simeon Bosco</t>
+  </si>
+  <si>
+    <t>Duncan Frami IV</t>
+  </si>
+  <si>
+    <t>Miss Carmella King DVM</t>
+  </si>
+  <si>
+    <t>Mohammad Wolff</t>
+  </si>
+  <si>
+    <t>Mr. Antone Beahan Jr.</t>
+  </si>
+  <si>
+    <t>Mrs. Palma Stracke</t>
+  </si>
+  <si>
+    <t>Malvina Stehr</t>
+  </si>
+  <si>
+    <t>Miss Abigale Corkery</t>
+  </si>
+  <si>
+    <t>Floyd Kub</t>
+  </si>
+  <si>
+    <t>Ms. Delpha Murphy</t>
+  </si>
+  <si>
+    <t>Dillan Wyman</t>
+  </si>
+  <si>
+    <t>Dr. Ole Gleichner DVM</t>
+  </si>
+  <si>
+    <t>Mrs. Daniela Gleason</t>
+  </si>
+  <si>
+    <t>Fredy Walsh</t>
+  </si>
+  <si>
+    <t>Laila Considine</t>
+  </si>
+  <si>
+    <t>Triston Bauch</t>
+  </si>
+  <si>
+    <t>Joel Turner II</t>
+  </si>
+  <si>
+    <t>Oswald Lubowitz Sr.</t>
+  </si>
+  <si>
+    <t>Margarete Hill</t>
+  </si>
+  <si>
+    <t>Emmy Bahringer</t>
+  </si>
+  <si>
+    <t>Prof. Pansy Johnson IV</t>
+  </si>
+  <si>
+    <t>Jailyn Hackett DVM</t>
+  </si>
+  <si>
+    <t>Phoebe Walker</t>
+  </si>
+  <si>
+    <t>Ray Corkery</t>
+  </si>
+  <si>
+    <t>Mr. Waylon Trantow</t>
+  </si>
+  <si>
+    <t>Prof. Dorian Barrows</t>
+  </si>
+  <si>
+    <t>Emmanuel Kris PhD</t>
+  </si>
+  <si>
+    <t>Lenna Prohaska</t>
+  </si>
+  <si>
+    <t>Miss Aliya Swaniawski</t>
+  </si>
+  <si>
+    <t>Antonio Beatty</t>
+  </si>
+  <si>
+    <t>Cooper Becker</t>
+  </si>
+  <si>
+    <t>Ben McKenzie DVM</t>
+  </si>
+  <si>
+    <t>Dr. Briana Weissnat DVM</t>
+  </si>
+  <si>
+    <t>Dr. Trisha McGlynn PhD</t>
+  </si>
+  <si>
+    <t>Valerie Osinski</t>
+  </si>
+  <si>
+    <t>Keanu Feest</t>
+  </si>
+  <si>
+    <t>Fannie Barton</t>
+  </si>
+  <si>
+    <t>Yoshiko Fritsch</t>
+  </si>
+  <si>
+    <t>Christian Kuhic</t>
+  </si>
+  <si>
+    <t>Ms. Carolyn Beer IV</t>
   </si>
 </sst>
 </file>

</xml_diff>